<commit_message>
Update diagnosis_tool.xlsx with new data
</commit_message>
<xml_diff>
--- a/diagnosis_tool.xlsx
+++ b/diagnosis_tool.xlsx
@@ -11,7 +11,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="92">
+  <si>
+    <t>年齢を教えてください</t>
+  </si>
+  <si>
+    <t>18-25歳,26-35歳,36-45歳,46歳以上</t>
+  </si>
+  <si>
+    <t>10,8,6,4</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Age and male fertility"</t>
+  </si>
+  <si>
+    <t>BMIを計算してください（体重kg / (身長m x 身長m)）</t>
+  </si>
+  <si>
+    <t>18.5未満：低体重,18.5 - 24.9：正常体重,25.0 - 29.9：過体重,30.0以上：肥満</t>
+  </si>
+  <si>
+    <t>3,10,6,0</t>
+  </si>
+  <si>
+    <t>論文タイトル: "BMI and its effects on male fertility"</t>
+  </si>
   <si>
     <t>果物や野菜はどのくらい食べていますか？</t>
   </si>
@@ -35,13 +59,241 @@
   </si>
   <si>
     <t>論文タイトル: "Impact of processed food consumption on male fertility"</t>
+  </si>
+  <si>
+    <t>マグロやイワシ、サンマ、サバなどの魚を食べていますか？</t>
+  </si>
+  <si>
+    <t>毎日摂取,週に3回以上,月に数回,ほとんど摂取しない</t>
+  </si>
+  <si>
+    <t>10,8,4,1</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Effect of omega-3 fatty acids on male fertility"</t>
+  </si>
+  <si>
+    <t>トマトやホウレンソウ、ピーマン、ブロッコリー、キウイ、柑橘類、イチゴなどを食べていますか？</t>
+  </si>
+  <si>
+    <t>日常的に摂取する,週に数回は摂取する,月に数回以下,ほとんど摂取しない</t>
+  </si>
+  <si>
+    <t>10,7,3,1</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Antioxidants and male fertility"</t>
+  </si>
+  <si>
+    <t>1週間にどのくらい運動していますか？</t>
+  </si>
+  <si>
+    <t>毎日運動する,週に4-6回,週に1-3回,ほとんど運動しない</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Physical activity and semen quality: A comprehensive review"</t>
+  </si>
+  <si>
+    <t>有酸素運動と筋トレのどちらを主にしますか？</t>
+  </si>
+  <si>
+    <t>両方をバランスよく行う,主に有酸素運動,主に筋トレ,運動しない</t>
+  </si>
+  <si>
+    <t>10,8,8,1</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Balanced exercise for male fertility: Effects on sperm parameters"</t>
+  </si>
+  <si>
+    <t>1日の平均睡眠時間は？</t>
+  </si>
+  <si>
+    <t>7-9時間,6-7時間,5-6時間,5時間未満</t>
+  </si>
+  <si>
+    <t>10,6,3,0</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Sleep duration and male fertility: An observational study"</t>
+  </si>
+  <si>
+    <t>睡眠の質はどうですか？</t>
+  </si>
+  <si>
+    <t>ほとんど中断されない,月に数回中断される,週に数回中断される,毎夜中断される</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Impact of interrupted sleep on male reproductive health"</t>
+  </si>
+  <si>
+    <t>就寝時間は規則的ですか？</t>
+  </si>
+  <si>
+    <t>毎夜同じ時間に床に就く,多くの夜は同じ時間,時々一貫性がある,不規則な睡眠スケジュール</t>
+  </si>
+  <si>
+    <t>10,7,4,1</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Regular sleep patterns and male fertility"</t>
+  </si>
+  <si>
+    <t>携帯電話を日常的に身につけていますか？</t>
+  </si>
+  <si>
+    <t>携帯電話を体から遠ざける、電磁波防護ケースを使用する,日常的には注意するが、完全ではない,たまにしか気にしない,常に体の近くに携帯電話を持っている</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Mobile phone radiation and its impact on sperm quality"</t>
+  </si>
+  <si>
+    <t>どんな下着を使用していますか？</t>
+  </si>
+  <si>
+    <t>ルーズな下着を使用する,時々タイトな下着を使用する,主にタイトな下着を使用する,常にタイトな下着を使用する</t>
+  </si>
+  <si>
+    <t>10,5,3,0</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Tight underwear and male fertility"</t>
+  </si>
+  <si>
+    <t>日々のストレスはどうですか？</t>
+  </si>
+  <si>
+    <t>ほとんど感じない,月に数回感じる,週に数回感じる,毎日感じる</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Stress levels and their impact on male reproductive hormones"</t>
+  </si>
+  <si>
+    <t>リラックスする方法・活動をしていますか？</t>
+  </si>
+  <si>
+    <t>毎日行う,週に数回行う,月に数回,全く行わない</t>
+  </si>
+  <si>
+    <t>10,7,4,0</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Relaxation techniques and their effects on male fertility"</t>
+  </si>
+  <si>
+    <t>ストレスにうまく対処して生活していますか？</t>
+  </si>
+  <si>
+    <t>効果的に管理している,まあまあ管理している,あまり管理できていない,全く管理できていない</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Stress coping mechanisms and sperm health"</t>
+  </si>
+  <si>
+    <t>喫煙していますか？</t>
+  </si>
+  <si>
+    <t>全く吸わない,以前は吸っていたがやめた,たまに吸う,定期的に吸う</t>
+  </si>
+  <si>
+    <t>10,7,2,-2</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Smoking and its effects on sperm DNA integrity"</t>
+  </si>
+  <si>
+    <t>お酒は飲みますか？</t>
+  </si>
+  <si>
+    <t>全く飲まない,月に数回,週に数回,毎日飲む</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Alcohol intake and its impact on male fertility"</t>
+  </si>
+  <si>
+    <t>育毛剤やステロイドを使っていますか？</t>
+  </si>
+  <si>
+    <t>使用していない,過去に使用したことがあるが現在は使用していない,たまに使用する,定期的に使用する</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Impact of medicated products on male fertility"</t>
+  </si>
+  <si>
+    <t>長時間座っていますか？</t>
+  </si>
+  <si>
+    <t>ほとんど座っていない,1-3時間座る,4-6時間座る,7時間以上座る</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Sedentary behavior and its effects on semen quality"</t>
+  </si>
+  <si>
+    <t>入浴していますか？</t>
+  </si>
+  <si>
+    <t>毎日シャワーを浴びる,週に数回浴槽に浸かる,毎日浴槽に浸かる,ほとんど浴槽に浸からない</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Heat exposure and sperm production"</t>
+  </si>
+  <si>
+    <t>サウナを利用していますか？</t>
+  </si>
+  <si>
+    <t>週に数回利用する,月に数回利用する,ほとんど利用しない,毎日利用する</t>
+  </si>
+  <si>
+    <t>1,5,10,1</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Sauna use and male fertility"</t>
+  </si>
+  <si>
+    <t>甘いものを食べていますか？</t>
+  </si>
+  <si>
+    <t>ほとんど摂取しない,月に数回,週に数回,毎日</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Sugar intake and male reproductive health"</t>
+  </si>
+  <si>
+    <t>サイクリングをしていますか？</t>
+  </si>
+  <si>
+    <t>サイクリングをしない,週に1-3時間,週に4-6時間,週に7時間以上</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Cycling frequency and its impact on male fertility"</t>
+  </si>
+  <si>
+    <t>どんな職業ですか？</t>
+  </si>
+  <si>
+    <t>環境リスクが低い、またはストレスが少ない仕事,重労働または体を動かす仕事,高温環境での作業,化学物質や有害物質に頻繁に触れる仕事</t>
+  </si>
+  <si>
+    <t>10,7,2,0</t>
+  </si>
+  <si>
+    <t>論文タイトル: "Occupational hazards and male fertility"</t>
+  </si>
+  <si>
+    <t>高温な作業環境での仕事はありますか？</t>
+  </si>
+  <si>
+    <t>高温環境での作業はしない,月に数回高温環境で作業する,週に数回高温環境で作業する,毎日高温環境で作業する</t>
+  </si>
+  <si>
+    <t>論文タイトル: "High temperature work environments and their effects on male fertility"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -51,6 +303,15 @@
     <font>
       <color rgb="FF0D0D0D"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color theme="1"/>
+      <name val="&quot;Google Sans Mono&quot;"/>
     </font>
   </fonts>
   <fills count="3">
@@ -73,12 +334,27 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -295,15 +571,20 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="42.63"/>
+    <col customWidth="1" min="2" max="2" width="44.0"/>
+    <col customWidth="1" min="4" max="4" width="57.75"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -314,14 +595,350 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>